<commit_message>
add: new function to generate guia
</commit_message>
<xml_diff>
--- a/output/bultos_pedido_collahuasi.xlsx
+++ b/output/bultos_pedido_collahuasi.xlsx
@@ -7,9 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Cajas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ASN" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="detalle" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Pallets" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cajas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ASN" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="detalle" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,17 +439,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Pallet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>LPN</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Peso (kg)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TipoCaja</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -470,25 +471,361 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SAL0000004524</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>7.29</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>GSP 4</t>
-        </is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SAL0000004097</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>40</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SAL0000004098</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SAL0000004099</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SAL0000004100</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SAL0000004102</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SAL0000004267</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SAL0000004267</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SAL0000004268</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SAL0000004269</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pallet2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SAL0000004245</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Pallet2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SAL0000004270</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Pallet2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SAL0000004271</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Pallet2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SAL0000004272</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Pallet2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SAL0000004273</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Pallet2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SAL0000004274</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -502,7 +839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,55 +850,81 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Tipo</t>
+          <t>LPN</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unidades</t>
+          <t>Peso (kg)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Peso(kg/unid)</t>
+          <t>TipoCaja</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Alto(cm/unid)</t>
+          <t>Alto (cm)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Ancho(cm/unid)</t>
+          <t>Largo (cm)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Largo(cm/unid)</t>
+          <t>Ancho (cm)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>SAL0000004101</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>GSP 4</t>
         </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>7.29</v>
       </c>
       <c r="D2" t="n">
         <v>36</v>
       </c>
       <c r="E2" t="n">
+        <v>56</v>
+      </c>
+      <c r="F2" t="n">
         <v>40</v>
       </c>
-      <c r="F2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SAL0000004275</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>55</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GSP 3</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="n">
         <v>56</v>
+      </c>
+      <c r="F3" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -575,7 +938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,59 +949,468 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LPN</t>
+          <t>Tipo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CodItem</t>
+          <t>Unidades</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>NomItem</t>
+          <t>Peso(kg/unid)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unidades</t>
+          <t>Alto(cm/unid)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Ancho(cm/unid)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Largo(cm/unid)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SAL0000004524</t>
+          <t>GSP 4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2140033</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STEITZ SECURA KST STAVANGER GTX AF NB 41</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SAL0000004524</t>
+          <t>GSP 3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2140038</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>55</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pallet</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pallet</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LPN</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CodItem</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NomItem</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unidades</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SAL0000004097</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SAL0000004098</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2140035</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>STEITZ SECURA KST STAVANGER GTX AF NB 46</t>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
         </is>
       </c>
       <c r="D3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SAL0000004099</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SAL0000004100</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SAL0000004101</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2140033</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 41</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SAL0000004102</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2140040</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 37</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SAL0000004245</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SAL0000004267</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2140033</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 41</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SAL0000004267</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SAL0000004268</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2140033</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 41</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SAL0000004269</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2140040</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 37</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SAL0000004270</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SAL0000004271</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SAL0000004272</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SAL0000004273</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SAL0000004274</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>SAL0000004275</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2140035</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>STEITZ SECURA KST STAVANGER GTX AF NB 43</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: creation big label and input protection
</commit_message>
<xml_diff>
--- a/output/bultos_pedido_collahuasi.xlsx
+++ b/output/bultos_pedido_collahuasi.xlsx
@@ -7,9 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Cajas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ASN" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="detalle" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Pallets" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cajas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ASN" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="detalle" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,17 +439,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Pallet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>LPN</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Peso (kg)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TipoCaja</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -470,145 +471,73 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>SAL0000004478</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>GSP 3</t>
-        </is>
-      </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SAL0000004491</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SAL0000004492</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>GSP 3</t>
-        </is>
-      </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SAL0000004492</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+          <t>Pallet1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SAL0000004494</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>GSP 3</t>
-        </is>
-      </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SAL0000004493</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>GSP 3</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" t="n">
-        <v>56</v>
-      </c>
-      <c r="F5" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>SAL0000004494</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>GSP 3</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>20</v>
-      </c>
-      <c r="E6" t="n">
-        <v>56</v>
-      </c>
-      <c r="F6" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SAL0000004528</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>GSP 3</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>20</v>
-      </c>
-      <c r="E7" t="n">
-        <v>56</v>
-      </c>
-      <c r="F7" t="n">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,55 +562,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Tipo</t>
+          <t>LPN</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unidades</t>
+          <t>Peso (kg)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Peso(kg/unid)</t>
+          <t>TipoCaja</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Alto(cm/unid)</t>
+          <t>Alto (cm)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Ancho(cm/unid)</t>
+          <t>Largo (cm)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Largo(cm/unid)</t>
+          <t>Ancho (cm)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>SAL0000004491</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>GSP 3</t>
         </is>
-      </c>
-      <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>20</v>
       </c>
       <c r="E2" t="n">
+        <v>56</v>
+      </c>
+      <c r="F2" t="n">
         <v>40</v>
       </c>
-      <c r="F2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SAL0000004493</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>22</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GSP 2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>31</v>
+      </c>
+      <c r="E3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SAL0000004528</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>GSP 3</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>20</v>
+      </c>
+      <c r="E4" t="n">
         <v>56</v>
+      </c>
+      <c r="F4" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -690,6 +669,145 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unidades</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Peso(kg/unid)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Alto(cm/unid)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Ancho(cm/unid)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Largo(cm/unid)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GSP 3</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GSP 2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" t="n">
+        <v>31</v>
+      </c>
+      <c r="E3" t="n">
+        <v>31</v>
+      </c>
+      <c r="F3" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GSP 3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20</v>
+      </c>
+      <c r="E4" t="n">
+        <v>40</v>
+      </c>
+      <c r="F4" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pallet</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>